<commit_message>
Adding more participants to sus scores
</commit_message>
<xml_diff>
--- a/Appendix/Sus Results/Sus Scores.xlsx
+++ b/Appendix/Sus Results/Sus Scores.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Participant 1</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Sus Grade</t>
+  </si>
+  <si>
+    <t>Participant 10</t>
   </si>
 </sst>
 </file>
@@ -191,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,13 +209,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +318,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -335,8 +332,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -346,33 +347,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -387,20 +361,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -733,12 +734,12 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -747,47 +748,47 @@
       <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:13" ht="18">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="18" t="s">
         <v>16</v>
       </c>
     </row>
@@ -827,37 +828,37 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="16">
-        <v>4</v>
-      </c>
-      <c r="C4" s="16">
-        <v>1</v>
-      </c>
-      <c r="D4" s="16">
-        <v>4</v>
-      </c>
-      <c r="E4" s="16">
-        <v>1</v>
-      </c>
-      <c r="F4" s="16">
-        <v>4</v>
-      </c>
-      <c r="G4" s="16">
-        <v>2</v>
-      </c>
-      <c r="H4" s="16">
-        <v>5</v>
-      </c>
-      <c r="I4" s="16">
-        <v>1</v>
-      </c>
-      <c r="J4" s="16">
-        <v>5</v>
-      </c>
-      <c r="K4" s="16">
+      <c r="A4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14">
+        <v>4</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>4</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1</v>
+      </c>
+      <c r="F4" s="14">
+        <v>4</v>
+      </c>
+      <c r="G4" s="14">
+        <v>2</v>
+      </c>
+      <c r="H4" s="14">
+        <v>5</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1</v>
+      </c>
+      <c r="J4" s="14">
+        <v>5</v>
+      </c>
+      <c r="K4" s="14">
         <v>1</v>
       </c>
     </row>
@@ -897,37 +898,37 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="16">
-        <v>4</v>
-      </c>
-      <c r="C6" s="16">
-        <v>2</v>
-      </c>
-      <c r="D6" s="16">
-        <v>4</v>
-      </c>
-      <c r="E6" s="16">
-        <v>1</v>
-      </c>
-      <c r="F6" s="16">
-        <v>5</v>
-      </c>
-      <c r="G6" s="16">
-        <v>1</v>
-      </c>
-      <c r="H6" s="16">
-        <v>5</v>
-      </c>
-      <c r="I6" s="16">
-        <v>3</v>
-      </c>
-      <c r="J6" s="16">
-        <v>4</v>
-      </c>
-      <c r="K6" s="16">
+      <c r="A6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2</v>
+      </c>
+      <c r="D6" s="14">
+        <v>4</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" s="14">
+        <v>5</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1</v>
+      </c>
+      <c r="H6" s="14">
+        <v>5</v>
+      </c>
+      <c r="I6" s="14">
+        <v>3</v>
+      </c>
+      <c r="J6" s="14">
+        <v>4</v>
+      </c>
+      <c r="K6" s="14">
         <v>1</v>
       </c>
     </row>
@@ -967,37 +968,37 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16">
-        <v>3</v>
-      </c>
-      <c r="C8" s="16">
-        <v>1</v>
-      </c>
-      <c r="D8" s="16">
-        <v>5</v>
-      </c>
-      <c r="E8" s="16">
-        <v>1</v>
-      </c>
-      <c r="F8" s="16">
-        <v>5</v>
-      </c>
-      <c r="G8" s="16">
-        <v>2</v>
-      </c>
-      <c r="H8" s="16">
-        <v>4</v>
-      </c>
-      <c r="I8" s="16">
-        <v>2</v>
-      </c>
-      <c r="J8" s="16">
-        <v>5</v>
-      </c>
-      <c r="K8" s="16">
+      <c r="A8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="14">
+        <v>3</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14">
+        <v>5</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14">
+        <v>5</v>
+      </c>
+      <c r="G8" s="14">
+        <v>2</v>
+      </c>
+      <c r="H8" s="14">
+        <v>4</v>
+      </c>
+      <c r="I8" s="14">
+        <v>2</v>
+      </c>
+      <c r="J8" s="14">
+        <v>5</v>
+      </c>
+      <c r="K8" s="14">
         <v>1</v>
       </c>
     </row>
@@ -1037,37 +1038,37 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="16">
-        <v>4</v>
-      </c>
-      <c r="C10" s="16">
-        <v>1</v>
-      </c>
-      <c r="D10" s="16">
-        <v>5</v>
-      </c>
-      <c r="E10" s="16">
-        <v>1</v>
-      </c>
-      <c r="F10" s="16">
-        <v>4</v>
-      </c>
-      <c r="G10" s="16">
-        <v>1</v>
-      </c>
-      <c r="H10" s="16">
-        <v>5</v>
-      </c>
-      <c r="I10" s="16">
-        <v>1</v>
-      </c>
-      <c r="J10" s="16">
-        <v>5</v>
-      </c>
-      <c r="K10" s="16">
+      <c r="B10" s="14">
+        <v>4</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1</v>
+      </c>
+      <c r="D10" s="14">
+        <v>5</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14">
+        <v>4</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1</v>
+      </c>
+      <c r="H10" s="14">
+        <v>5</v>
+      </c>
+      <c r="I10" s="14">
+        <v>1</v>
+      </c>
+      <c r="J10" s="14">
+        <v>5</v>
+      </c>
+      <c r="K10" s="14">
         <v>1</v>
       </c>
     </row>
@@ -1107,17 +1108,39 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="A12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="14">
+        <v>5</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2</v>
+      </c>
+      <c r="D12" s="14">
+        <v>5</v>
+      </c>
+      <c r="E12" s="14">
+        <v>2</v>
+      </c>
+      <c r="F12" s="14">
+        <v>4</v>
+      </c>
+      <c r="G12" s="14">
+        <v>3</v>
+      </c>
+      <c r="H12" s="14">
+        <v>4</v>
+      </c>
+      <c r="I12" s="14">
+        <v>1</v>
+      </c>
+      <c r="J12" s="14">
+        <v>4</v>
+      </c>
+      <c r="K12" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1"/>
@@ -1146,58 +1169,58 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:13" ht="25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="18">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="14" t="s">
+      <c r="L16" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1236,7 +1259,7 @@
         <v>4</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" ref="L17:L25" si="0">SUM(B17:K17)*2.5</f>
+        <f t="shared" ref="L17:L26" si="0">SUM(B17:K17)*2.5</f>
         <v>87.5</v>
       </c>
       <c r="M17" s="3" t="s">
@@ -1244,44 +1267,44 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="9">
-        <v>3</v>
-      </c>
-      <c r="C18" s="9">
-        <v>4</v>
-      </c>
-      <c r="D18" s="9">
-        <v>3</v>
-      </c>
-      <c r="E18" s="9">
-        <v>4</v>
-      </c>
-      <c r="F18" s="9">
-        <v>3</v>
-      </c>
-      <c r="G18" s="9">
-        <v>3</v>
-      </c>
-      <c r="H18" s="9">
-        <v>4</v>
-      </c>
-      <c r="I18" s="9">
-        <v>1</v>
-      </c>
-      <c r="J18" s="9">
-        <v>4</v>
-      </c>
-      <c r="K18" s="9">
-        <v>4</v>
-      </c>
-      <c r="L18" s="10">
+      <c r="A18" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="21">
+        <v>3</v>
+      </c>
+      <c r="C18" s="21">
+        <v>4</v>
+      </c>
+      <c r="D18" s="21">
+        <v>3</v>
+      </c>
+      <c r="E18" s="21">
+        <v>4</v>
+      </c>
+      <c r="F18" s="21">
+        <v>3</v>
+      </c>
+      <c r="G18" s="21">
+        <v>3</v>
+      </c>
+      <c r="H18" s="21">
+        <v>4</v>
+      </c>
+      <c r="I18" s="21">
+        <v>1</v>
+      </c>
+      <c r="J18" s="21">
+        <v>4</v>
+      </c>
+      <c r="K18" s="21">
+        <v>4</v>
+      </c>
+      <c r="L18" s="22">
         <f t="shared" si="0"/>
         <v>82.5</v>
       </c>
-      <c r="M18" s="9" t="s">
+      <c r="M18" s="21" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1328,44 +1351,44 @@
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="6">
-        <v>3</v>
-      </c>
-      <c r="C20" s="6">
-        <v>3</v>
-      </c>
-      <c r="D20" s="6">
-        <v>3</v>
-      </c>
-      <c r="E20" s="6">
-        <v>4</v>
-      </c>
-      <c r="F20" s="6">
-        <v>4</v>
-      </c>
-      <c r="G20" s="6">
-        <v>4</v>
-      </c>
-      <c r="H20" s="6">
-        <v>4</v>
-      </c>
-      <c r="I20" s="6">
-        <v>3</v>
-      </c>
-      <c r="J20" s="6">
-        <v>3</v>
-      </c>
-      <c r="K20" s="6">
-        <v>4</v>
-      </c>
-      <c r="L20" s="7">
+      <c r="A20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="14">
+        <v>3</v>
+      </c>
+      <c r="C20" s="14">
+        <v>3</v>
+      </c>
+      <c r="D20" s="14">
+        <v>3</v>
+      </c>
+      <c r="E20" s="14">
+        <v>4</v>
+      </c>
+      <c r="F20" s="14">
+        <v>4</v>
+      </c>
+      <c r="G20" s="14">
+        <v>4</v>
+      </c>
+      <c r="H20" s="14">
+        <v>4</v>
+      </c>
+      <c r="I20" s="14">
+        <v>3</v>
+      </c>
+      <c r="J20" s="14">
+        <v>3</v>
+      </c>
+      <c r="K20" s="14">
+        <v>4</v>
+      </c>
+      <c r="L20" s="23">
         <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="M20" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1412,44 +1435,44 @@
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="6">
-        <v>2</v>
-      </c>
-      <c r="C22" s="6">
-        <v>4</v>
-      </c>
-      <c r="D22" s="6">
-        <v>4</v>
-      </c>
-      <c r="E22" s="6">
-        <v>4</v>
-      </c>
-      <c r="F22" s="6">
-        <v>4</v>
-      </c>
-      <c r="G22" s="6">
-        <v>3</v>
-      </c>
-      <c r="H22" s="6">
-        <v>3</v>
-      </c>
-      <c r="I22" s="6">
-        <v>2</v>
-      </c>
-      <c r="J22" s="6">
-        <v>4</v>
-      </c>
-      <c r="K22" s="6">
-        <v>4</v>
-      </c>
-      <c r="L22" s="7">
+      <c r="A22" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="14">
+        <v>2</v>
+      </c>
+      <c r="C22" s="14">
+        <v>4</v>
+      </c>
+      <c r="D22" s="14">
+        <v>4</v>
+      </c>
+      <c r="E22" s="14">
+        <v>4</v>
+      </c>
+      <c r="F22" s="14">
+        <v>4</v>
+      </c>
+      <c r="G22" s="14">
+        <v>3</v>
+      </c>
+      <c r="H22" s="14">
+        <v>3</v>
+      </c>
+      <c r="I22" s="14">
+        <v>2</v>
+      </c>
+      <c r="J22" s="14">
+        <v>4</v>
+      </c>
+      <c r="K22" s="14">
+        <v>4</v>
+      </c>
+      <c r="L22" s="23">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="M22" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1496,44 +1519,44 @@
       </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="6">
-        <v>4</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-      <c r="D24" s="6">
-        <v>5</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6">
-        <v>4</v>
-      </c>
-      <c r="G24" s="6">
-        <v>1</v>
-      </c>
-      <c r="H24" s="6">
-        <v>5</v>
-      </c>
-      <c r="I24" s="6">
-        <v>1</v>
-      </c>
-      <c r="J24" s="6">
-        <v>5</v>
-      </c>
-      <c r="K24" s="6">
-        <v>1</v>
-      </c>
-      <c r="L24" s="7">
+      <c r="B24" s="14">
+        <v>4</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
+      <c r="D24" s="14">
+        <v>5</v>
+      </c>
+      <c r="E24" s="14">
+        <v>1</v>
+      </c>
+      <c r="F24" s="14">
+        <v>4</v>
+      </c>
+      <c r="G24" s="14">
+        <v>1</v>
+      </c>
+      <c r="H24" s="14">
+        <v>5</v>
+      </c>
+      <c r="I24" s="14">
+        <v>1</v>
+      </c>
+      <c r="J24" s="14">
+        <v>5</v>
+      </c>
+      <c r="K24" s="14">
+        <v>1</v>
+      </c>
+      <c r="L24" s="23">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="M24" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1579,23 +1602,65 @@
         <v>18</v>
       </c>
     </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="14">
+        <v>5</v>
+      </c>
+      <c r="C26" s="14">
+        <v>2</v>
+      </c>
+      <c r="D26" s="14">
+        <v>5</v>
+      </c>
+      <c r="E26" s="14">
+        <v>2</v>
+      </c>
+      <c r="F26" s="14">
+        <v>4</v>
+      </c>
+      <c r="G26" s="14">
+        <v>3</v>
+      </c>
+      <c r="H26" s="14">
+        <v>4</v>
+      </c>
+      <c r="I26" s="14">
+        <v>1</v>
+      </c>
+      <c r="J26" s="14">
+        <v>4</v>
+      </c>
+      <c r="K26" s="14">
+        <v>1</v>
+      </c>
+      <c r="L26" s="23">
+        <f t="shared" si="0"/>
+        <v>77.5</v>
+      </c>
+      <c r="M26" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="29" spans="1:13" ht="18">
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="20"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="7"/>
     </row>
     <row r="30" spans="1:13">
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="1"/>
@@ -1607,10 +1672,10 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="22"/>
+      <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="1"/>
@@ -1622,22 +1687,22 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="22"/>
+      <c r="L31" s="9"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="25"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>